<commit_message>
Adding tutorial part 3
</commit_message>
<xml_diff>
--- a/learn_everyday.xlsx
+++ b/learn_everyday.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Subclass</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>example_machine_learning.py</t>
+  </si>
+  <si>
+    <t>Machine Learning Crash Course: Part 4</t>
+  </si>
+  <si>
+    <t>https://ml.berkeley.edu/blog/2017/07/13/tutorial-4/</t>
   </si>
 </sst>
 </file>
@@ -444,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03CA27F-C63C-47C2-8C3D-E7D485C49C39}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,29 +534,45 @@
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="D5" s="2">
+        <v>43080</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="2">
         <v>43079</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EE0C2F6C-F864-4E54-B666-4DC8B7615058}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{3483E081-1E82-4986-B98E-B283B4136290}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>